<commit_message>
MTR v3 - updated references
</commit_message>
<xml_diff>
--- a/Mid-Thesis Report/MTR References v2.xlsx
+++ b/Mid-Thesis Report/MTR References v2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9D1E1523-4A19-4032-A130-96A059553BD6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1418BB44-AC05-45D2-B1B3-D81B16C024CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11070" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12075" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature Review" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -672,12 +672,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -771,13 +765,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1955,9 +1949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC32EA15-C31D-47DB-A246-87AD187AAB11}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
MTR v4 - updated references
</commit_message>
<xml_diff>
--- a/Mid-Thesis Report/MTR References v2.xlsx
+++ b/Mid-Thesis Report/MTR References v2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1418BB44-AC05-45D2-B1B3-D81B16C024CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A3DF15D-D980-41DF-B5E8-2D401BD77275}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12075" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13080" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature Review" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="126">
   <si>
     <t>Sno</t>
   </si>
@@ -407,12 +407,6 @@
 Contract, OnlineSecurity, TechSupport, Tenure &amp; DeviceProtection</t>
   </si>
   <si>
-    <t>Phase 1: Variance Analysis, Correlation Matrix, Outliers Removed
-Phase 2: Cleaning &amp; Filtering
-Phase 3: Feature Selection using Gravitational Search Algorithm
-Feature Importance</t>
-  </si>
-  <si>
     <t>Accuracy: 
 Logistic Regression - 97.8%
 Decision Tree - 78.3%
@@ -430,12 +424,6 @@
 Decision Trees - 73.05%
 K-Nearest Neigbor - 79.86%
 Artifical Neural Network - 82.83%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label Encoding Binary Columns, Scaling Numerical Columns, 
-Feature Importance result:
-Contract_month-to-month, tenure, InternetService_FiberOptic
-</t>
   </si>
   <si>
     <t>AUC:
@@ -494,12 +482,6 @@
 Best model: log-normal model</t>
   </si>
   <si>
-    <t>Feature Selection using CorrelationMatrix Operator
-Total Charges is discarded
-RapidMiner is used to do feature selection:
-Contract, OnlineSecurity, TechSupport, Tenure &amp; DeviceProtection</t>
-  </si>
-  <si>
     <t>AUC:
 Gradient Boosted Trees (before oversampling) - 0.834
 Gradient Boosted Trees (after oversampling) - 0.865
@@ -520,10 +502,6 @@
     <t>Logistic Regression:
 Accuracy - 76.7%
 AUC - 0.767</t>
-  </si>
-  <si>
-    <t>Top 5 Significant features:
-FiberOptic, MonthToMonthContract, DSL, OneYearContract, StreamingMovies</t>
   </si>
   <si>
     <t>An Effective Classifier for Predicting Churn in Telecommunication</t>
@@ -594,12 +572,94 @@
   <si>
     <t xml:space="preserve">One Hot Encoding </t>
   </si>
+  <si>
+    <t>Phase 1: 
+Variance Analysis, 
+Correlation Matrix, 
+Outliers Removed
+Phase 2: 
+Cleaning &amp; Filtering
+Phase 3: 
+Feature Selection using Gravitational Search Algorithm
+Feature Importance</t>
+  </si>
+  <si>
+    <t>Tokenization, 
+Standardization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label Encoding Binary Columns,
+Scaling Numerical Columns, 
+Feature Importance result:
+Contract_month-to-month, tenure, InternetService_FiberOptic
+</t>
+  </si>
+  <si>
+    <t>Top 5 Significant features using Feature Selection:
+- FiberOptic
+- MonthToMonthContract
+- DSL
+- OneYearContract
+- StreamingMovies</t>
+  </si>
+  <si>
+    <t>Feature Selection using 
+CorrelationMatrix Operator
+Total Charges is discarded
+RapidMiner is used to do feature selection:
+Contract, OnlineSecurity, 
+TechSupport, Tenure &amp; 
+DeviceProtection</t>
+  </si>
+  <si>
+    <t>PMM -
+Predictive Mean Matching</t>
+  </si>
+  <si>
+    <t>(Tamuka and Sibanda, 2021)</t>
+  </si>
+  <si>
+    <t>(Lalwani et al., 2021)</t>
+  </si>
+  <si>
+    <t>(Momin et al., 2020)</t>
+  </si>
+  <si>
+    <t>(Oka and Arifin, 2020)</t>
+  </si>
+  <si>
+    <t>(Mahdi et al., 2020)</t>
+  </si>
+  <si>
+    <t>(Ebrah and Elnasir, 2019)</t>
+  </si>
+  <si>
+    <t>(Havrylovych and Nataliia Kuznietsova, 2019)</t>
+  </si>
+  <si>
+    <t>(Halibas et al., 2019)</t>
+  </si>
+  <si>
+    <t>(Kriti, 2019)</t>
+  </si>
+  <si>
+    <t>(Hargreaves, 2019)</t>
+  </si>
+  <si>
+    <t>(Pamina et al., 2019)</t>
+  </si>
+  <si>
+    <t>(Induja and Eswaramurthy, 2015)</t>
+  </si>
+  <si>
+    <t>(Agrawal, 2018)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +691,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +742,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -703,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -766,13 +839,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1059,7 +1147,7 @@
     <sheetView zoomScale="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,18 +2038,18 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F14"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13" style="28" customWidth="1"/>
+    <col min="4" max="4" width="5" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1972,7 +2060,7 @@
       <c r="B1" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="26" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="13" t="s">
@@ -1986,235 +2074,261 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="21">
+      <c r="C2" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="23">
         <v>2021</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>90</v>
+      <c r="F2" s="21" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="27" t="s">
+        <v>114</v>
+      </c>
       <c r="D3" s="23">
         <v>2021</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>93</v>
+      <c r="E3" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="27" t="s">
+        <v>115</v>
+      </c>
       <c r="D4" s="23">
         <v>2020</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>91</v>
+      <c r="E4" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="D5" s="23">
         <v>2020</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+    </row>
+    <row r="6" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="27" t="s">
+        <v>117</v>
+      </c>
       <c r="D6" s="23">
         <v>2020</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>95</v>
+      <c r="E6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="27" t="s">
+        <v>118</v>
+      </c>
       <c r="D7" s="23">
         <v>2019</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>96</v>
+      <c r="E7" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="27" t="s">
+        <v>119</v>
+      </c>
       <c r="D8" s="23">
         <v>2019</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22" t="s">
-        <v>98</v>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="27" t="s">
+        <v>120</v>
+      </c>
       <c r="D9" s="23">
         <v>2019</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>100</v>
+      <c r="E9" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="27" t="s">
+        <v>121</v>
+      </c>
       <c r="D10" s="23">
         <v>2019</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="E10" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="27" t="s">
+        <v>122</v>
+      </c>
       <c r="D11" s="23">
         <v>2019</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>103</v>
+      <c r="E11" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="23"/>
+      <c r="B12" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>123</v>
+      </c>
       <c r="D12" s="23">
         <v>2019</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="E12" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="27" t="s">
+        <v>124</v>
+      </c>
       <c r="D13" s="23">
         <v>2019</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="F13" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="27" t="s">
+        <v>125</v>
+      </c>
       <c r="D14" s="23">
         <v>2018</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>109</v>
+      <c r="E14" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MTR v5 - 2.4 Class Imbalance
</commit_message>
<xml_diff>
--- a/Mid-Thesis Report/MTR References v2.xlsx
+++ b/Mid-Thesis Report/MTR References v2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A3DF15D-D980-41DF-B5E8-2D401BD77275}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{06298614-D26C-47BA-9BF6-79E7BC241D0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14085" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature Review" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -787,9 +787,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -802,18 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,15 +808,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -861,6 +837,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,10 +1135,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,45 +1150,45 @@
     <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="30" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>4</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>2021</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1209,7 +1200,7 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="25" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1221,10 +1212,10 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="10">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>2021</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1247,7 +1238,7 @@
       <c r="A4" s="3">
         <v>6</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2021</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1259,7 +1250,7 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="25" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1272,10 +1263,10 @@
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>2020</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1284,7 +1275,7 @@
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="25" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1294,446 +1285,446 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="10">
         <v>7</v>
       </c>
       <c r="B6" s="7">
         <v>2020</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="10">
         <v>8</v>
       </c>
       <c r="B7" s="7">
         <v>2020</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <v>9</v>
       </c>
       <c r="B8" s="7">
         <v>2020</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>10</v>
       </c>
       <c r="B9" s="7">
         <v>2020</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="7">
         <v>2019</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>11</v>
       </c>
       <c r="B11" s="7">
         <v>2019</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <v>12</v>
       </c>
       <c r="B12" s="7">
         <v>2019</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="21">
         <v>13</v>
       </c>
       <c r="B13" s="7">
         <v>2019</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>14</v>
       </c>
       <c r="B14" s="7">
         <v>2019</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="3">
         <v>15</v>
       </c>
       <c r="B15" s="7">
         <v>2019</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="22">
         <v>16</v>
       </c>
       <c r="B16" s="7">
         <v>2019</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="3">
         <v>17</v>
       </c>
       <c r="B17" s="7">
         <v>2019</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="22">
         <v>18</v>
       </c>
       <c r="B18" s="7">
         <v>2019</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="23">
         <v>22</v>
       </c>
       <c r="B19" s="7">
         <v>2019</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="7">
         <v>2018</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="23">
         <v>20</v>
       </c>
       <c r="B21" s="7">
         <v>2018</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>2018</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+      <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="7">
         <v>2017</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
+      <c r="F23" s="24"/>
+      <c r="G23" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17" t="s">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24" xr:uid="{D45BD7D7-215A-47F7-966D-3F456C2E73D0}">
@@ -1767,34 +1758,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="14">
+      <c r="C2" s="12"/>
+      <c r="D2" s="9">
         <v>2021</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1805,14 +1796,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12">
         <v>2021</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1823,14 +1814,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12">
         <v>2020</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1841,14 +1832,14 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12">
         <v>2020</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1859,14 +1850,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12">
         <v>2020</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1877,14 +1868,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12">
         <v>2019</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1895,14 +1886,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12">
         <v>2019</v>
       </c>
       <c r="E8" s="3"/>
@@ -1911,14 +1902,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="210" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12">
         <v>2019</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1929,64 +1920,64 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12">
         <v>2019</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12">
         <v>2019</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12">
         <v>2019</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12">
         <v>2019</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1997,28 +1988,28 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12">
         <v>2018</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12">
         <v>2018</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -2037,297 +2028,297 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC32EA15-C31D-47DB-A246-87AD187AAB11}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13" style="28" customWidth="1"/>
-    <col min="4" max="4" width="5" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="20" customWidth="1"/>
+    <col min="4" max="4" width="5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="15">
         <v>2021</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="15">
         <v>2021</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="15">
         <v>2020</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="15">
         <v>2020</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="15">
         <v>2020</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="15">
         <v>2019</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="15">
         <v>2019</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="15">
         <v>2019</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="15">
         <v>2019</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="15">
         <v>2019</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="15">
         <v>2019</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="13" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="15">
         <v>2019</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="15">
         <v>2018</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="13" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>